<commit_message>
Added practice MySQL and Mongodb database connection with python
</commit_message>
<xml_diff>
--- a/MySQL and Mongodb Queries.xlsx
+++ b/MySQL and Mongodb Queries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ganeshsha\Desktop\PPP\Mongodb and MySQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ganeshsha\Desktop\PPP\MySQL-and-Mongodb-Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C9BC19-B789-48A3-99AD-147AE19FC72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A23825-A101-4FC2-A361-F5E739ABA344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="255" yWindow="135" windowWidth="20235" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -76,11 +76,6 @@
     <t>Creates database in mysql with name mydatabase</t>
   </si>
   <si>
-    <t>mycursor.execute("SHOW DATABASE")
-for x in mycursor:
-        print(x)</t>
-  </si>
-  <si>
     <t>Connecting to a given database schema while connecting to mysql</t>
   </si>
   <si>
@@ -374,6 +369,14 @@
     </r>
   </si>
   <si>
+    <t>Python: Go to cmd and type: where python
+Mysql: Search for mysql workbench. Login to local host (or) write a python code to import mysql.coonector and execte it.</t>
+  </si>
+  <si>
+    <t>Mongodb: Open mongodb compass &gt; Click "Fill in connection fields individually" &gt; Connect.
+If throws error: Start &gt; Services &gt; Search for Mongodb Server and select &gt; click start. Then connect the localhost in mongodb compass</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">pip install mysql.connector  OR
 </t>
@@ -399,23 +402,21 @@
       </rPr>
       <t xml:space="preserve"> OR
 pip install mysql.connector-python-rf
+To check whether connector got installed or not. Use pip list in cmd
 </t>
     </r>
   </si>
   <si>
-    <t>Python: Go to cmd and type: where python
-Mysql: Search for mysql workbench. Login to local host (or) write a python code to import mysql.coonector and execte it.</t>
-  </si>
-  <si>
-    <t>Mongodb: Open mongodb compass &gt; Click "Fill in connection fields individually" &gt; Connect.
-If throws error: Start &gt; Services &gt; Search for Mongodb Server and select &gt; click start. Then connect the localhost in mongodb compass</t>
+    <t>mycursor.execute("SHOW DATABASES")
+for x in mycursor:
+        print(x)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,12 +437,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000CD"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -497,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -518,7 +513,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,8 +796,8 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,39 +814,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -866,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -874,13 +868,13 @@
     </row>
     <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -898,132 +892,132 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>64</v>
+        <v>19</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1074,74 +1068,74 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added practical creation of table collection in MYSQL and Mongodb with python
</commit_message>
<xml_diff>
--- a/MySQL and Mongodb Queries.xlsx
+++ b/MySQL and Mongodb Queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ganeshsha\Desktop\PPP\MySQL-and-Mongodb-Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A23825-A101-4FC2-A361-F5E739ABA344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2681898B-57FE-45E0-BC8A-C757B05D143F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="135" windowWidth="20235" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Description</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Connecting to a given database schema while connecting to mysql</t>
-  </si>
-  <si>
-    <t>Establishing connection to mysql database</t>
   </si>
   <si>
     <t>mydb = mysql.connector.connect(
@@ -95,10 +92,6 @@
   </si>
   <si>
     <t>Check if table exists</t>
-  </si>
-  <si>
-    <t>Mention the database name while establishing connection to mysql databale schema
-mycursor.execute("CREATE TABLE customers (name VARCHAR(255), address VARCHAR(255))")</t>
   </si>
   <si>
     <t>mycursor.execute("SHOW TABLES")
@@ -411,12 +404,95 @@
 for x in mycursor:
         print(x)</t>
   </si>
+  <si>
+    <t>Establishing connection</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MYSQL:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) Create table - For data types and widh details please refer online. Basically 3 datatypes.
+"""</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Note from stackoverflow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Display width doesn't change storage requirements for a data type.
+Display width doesn't alter the actual data in any way (ie: it stores the entire value for the data)
+A column returns it's full value when called in a query, regardless of the display width (the book directly contradicts this claim it makes as seen above)
+"""</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mention the database name while establishing connection to mysql databale schema
+mycursor.execute(
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CREATE TABLE friends (id INT AUTO_INCREMENT PRIMARY KEY, name VARCHAR(255), email VARCHAR(255), mobile INT)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"
+)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +525,15 @@
       <color rgb="FFA52A2A"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -796,8 +881,8 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,39 +899,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -860,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -868,13 +953,13 @@
     </row>
     <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -894,13 +979,13 @@
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -912,7 +997,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
@@ -923,101 +1008,103 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1068,74 +1155,74 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added practical insert queries
</commit_message>
<xml_diff>
--- a/MySQL and Mongodb Queries.xlsx
+++ b/MySQL and Mongodb Queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ganeshsha\Desktop\PPP\MySQL-and-Mongodb-Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2681898B-57FE-45E0-BC8A-C757B05D143F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670DBECF-D3DD-4DF2-A56A-6E0C0D77951B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="135" windowWidth="20235" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>Description</t>
   </si>
@@ -138,17 +138,6 @@
     <t>Insert multiple rows to a table</t>
   </si>
   <si>
-    <t>sql = "INSERT INTO customers (name, address) VALUES (%s, %s)"
-val = [
-  ('Peter', 'Lowstreet 4'),
-  ('Amy', 'Apple st 652'),
-]
-mycursor.executemany(sql, val)
-mydb.commit()
-print(mycursor.rowcount, "was inserted.")
-print("1 record inserted, ID:", mycursor.lastrowid)</t>
-  </si>
-  <si>
     <t>Checking if a database exists</t>
   </si>
   <si>
@@ -183,15 +172,6 @@
   </si>
   <si>
     <t>data types in database</t>
-  </si>
-  <si>
-    <t>Numeric</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>temporal</t>
   </si>
   <si>
     <t>deleting data from db(column and row, table)</t>
@@ -486,6 +466,45 @@
       <t>"
 )</t>
     </r>
+  </si>
+  <si>
+    <t>MYSQL: More topics to explore on Alter table.
+# Alter table name
+# Alter column name  
+# Alter table - add column
+# Alter table - delete column</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Numeric, String, Data time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTER Table </t>
+  </si>
+  <si>
+    <t># Alter table name
+# Alter column name  
+# Alter table - add column
+# Alter table - delete column</t>
+  </si>
+  <si>
+    <t>mycursor.rowcount</t>
+  </si>
+  <si>
+    <t>mycursor.fetchone</t>
+  </si>
+  <si>
+    <t>Explore mycursor methods</t>
+  </si>
+  <si>
+    <t>sql = "INSERT INTO friends (name, email, mobile) VALUES (%s,%s,%s)"
+val = ('Aditya', 'aditya@gmail.com', '99999')
+mycursor.execute(sql,val)
+mydb.commit()
+mycursor.rowcount
+print("1 record inserted, ID:", mycursor.lastrowid)</t>
   </si>
 </sst>
 </file>
@@ -577,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -598,6 +617,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,8 +903,8 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,39 +921,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -945,7 +967,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -953,13 +975,13 @@
     </row>
     <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -979,13 +1001,13 @@
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -997,7 +1019,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
@@ -1018,13 +1040,13 @@
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1047,7 +1069,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -1055,7 +1077,9 @@
         <v>22</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1069,42 +1093,42 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1141,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96533BAE-3066-4444-8E60-960485C90594}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,74 +1179,97 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>41</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Select and find prctical files
</commit_message>
<xml_diff>
--- a/MySQL and Mongodb Queries.xlsx
+++ b/MySQL and Mongodb Queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ganeshsha\Desktop\PPP\MySQL-and-Mongodb-Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670DBECF-D3DD-4DF2-A56A-6E0C0D77951B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C6E96A-94EB-4808-8EDB-7F6E97E678AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="135" windowWidth="20235" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>Description</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Create a table</t>
   </si>
   <si>
-    <t>Check if table exists</t>
-  </si>
-  <si>
     <t>mycursor.execute("SHOW TABLES")
 for x in mycursor:
         print(x)</t>
@@ -120,13 +117,6 @@
   </si>
   <si>
     <t>mycursor.execute("ALTER TABLE customers ADD COLUMN id INT AUTO_INCREMENT PRIMARY KEY")</t>
-  </si>
-  <si>
-    <t>sql = "INSERT INTO customers (name, address) VALUES (%s, %s)"
-val = ("John", "Highway 21")
-mycursor.execute(sql, val)
-mydb.commit()
-print(mycursor.rowcount, "record inserted.")</t>
   </si>
   <si>
     <t>Notice the statement: mydb.commit(). It is required to make the changes, otherwise no changes are made to the table.</t>
@@ -499,12 +489,43 @@
     <t>Explore mycursor methods</t>
   </si>
   <si>
+    <t>mydb1 = myclient['local']
+for col in mydb1.list_collection_names():
+    print(col)</t>
+  </si>
+  <si>
+    <t>Check if table or collection exists</t>
+  </si>
+  <si>
+    <t>mydb = myclient["mydatabase"]
+mycol = mydb["friends"]
+mydict = {"name":"Aditya, "email":"aditya@gmail.com, "mobile":"99999"}
+mydoc = mycol.insert_one(mydict)</t>
+  </si>
+  <si>
     <t>sql = "INSERT INTO friends (name, email, mobile) VALUES (%s,%s,%s)"
 val = ('Aditya', 'aditya@gmail.com', '99999')
 mycursor.execute(sql,val)
 mydb.commit()
 mycursor.rowcount
-print("1 record inserted, ID:", mycursor.lastrowid)</t>
+mycursor.lastrowid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+sql = "INSERT INTO friends (name, email, mobile) VALUES (%s, %s, %s)"
+val = [
+    ('Ravi', 'Ravi@gmail.com', '99998'),
+    ('Teja', 'aditya@gmail.com', '99997')
+]
+mycursor.executemany(sql,val)
+mydb.commit(</t>
+  </si>
+  <si>
+    <t>mydict =[
+    {'name':'Ravi', 'email':'Ravi@gmail.com', 'mobile':"99998"},
+    {'name':'Teja', 'email':'Teja@gmail.com', 'mobile':"99997"}
+]
+mydoc = mycol.insert_many(mydict)</t>
   </si>
 </sst>
 </file>
@@ -596,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -616,7 +637,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -903,8 +923,8 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,39 +941,39 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -967,7 +987,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -975,13 +995,13 @@
     </row>
     <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -1001,13 +1021,13 @@
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -1018,8 +1038,8 @@
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>55</v>
+      <c r="C8" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
@@ -1040,95 +1060,101 @@
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="B15" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1179,97 +1205,97 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>